<commit_message>
Correção dos gráficos do subtema "Energia" do tema "Meio Ambiente"
</commit_message>
<xml_diff>
--- a/data/Energia_Eletrica_Coelba.xlsx
+++ b/data/Energia_Eletrica_Coelba.xlsx
@@ -16,14 +16,14 @@
     <t>Ano</t>
   </si>
   <si>
-    <t>Consumo de energia elétrica do município (Kwh)</t>
+    <t>Consumo de energia elétrica do município (Mwh)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -33,29 +33,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7EFE4"/>
-        <bgColor rgb="FFF7EFE4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,18 +48,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,112 +283,112 @@
       <c r="A2" s="1">
         <v>2001.0</v>
       </c>
-      <c r="B2" s="2">
-        <v>2.229861974E9</v>
+      <c r="B2" s="1">
+        <v>2229861.974</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
         <v>2002.0</v>
       </c>
-      <c r="B3" s="2">
-        <v>2.156881062E9</v>
+      <c r="B3" s="1">
+        <v>2156881.062</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>2003.0</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.310499377E9</v>
+      <c r="B4" s="1">
+        <v>2310499.377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
         <v>2004.0</v>
       </c>
-      <c r="B5" s="2">
-        <v>2.149158339E9</v>
+      <c r="B5" s="1">
+        <v>2149158.339</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
         <v>2005.0</v>
       </c>
-      <c r="B6" s="2">
-        <v>2.503969005E9</v>
+      <c r="B6" s="1">
+        <v>2503969.005</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
         <v>2006.0</v>
       </c>
-      <c r="B7" s="2">
-        <v>2.558611402E9</v>
+      <c r="B7" s="1">
+        <v>2558611.402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
         <v>2007.0</v>
       </c>
-      <c r="B8" s="2">
-        <v>2.763375536E9</v>
+      <c r="B8" s="1">
+        <v>2763375.536</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
         <v>2008.0</v>
       </c>
-      <c r="B9" s="2">
-        <v>3.33292929E9</v>
+      <c r="B9" s="1">
+        <v>3332929.29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
         <v>2009.0</v>
       </c>
-      <c r="B10" s="2">
-        <v>3.528512546E9</v>
+      <c r="B10" s="1">
+        <v>3528512.546</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
         <v>2010.0</v>
       </c>
-      <c r="B11" s="2">
-        <v>3.288508268E9</v>
+      <c r="B11" s="1">
+        <v>3288508.268</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>2011.0</v>
       </c>
-      <c r="B12" s="2">
-        <v>3.703796797E9</v>
+      <c r="B12" s="1">
+        <v>3703796.797</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
         <v>2012.0</v>
       </c>
-      <c r="B13" s="2">
-        <v>3.604938748E9</v>
+      <c r="B13" s="1">
+        <v>3604938.748</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>2013.0</v>
       </c>
-      <c r="B14" s="3">
-        <v>3.804952547E9</v>
+      <c r="B14" s="1">
+        <v>3804952.547</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
         <v>2014.0</v>
       </c>
-      <c r="B15" s="2">
-        <v>3.891813401E9</v>
+      <c r="B15" s="1">
+        <v>3891813.401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>